<commit_message>
Corrección de BOM del Poncho Osciloscopio.
</commit_message>
<xml_diff>
--- a/Osciloscopio/fabricacion1/BOM.xlsx
+++ b/Osciloscopio/fabricacion1/BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="526" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KiCost" sheetId="1" state="visible" r:id="rId2"/>
@@ -411,7 +411,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="156">
   <si>
     <t>Board Qty:</t>
   </si>
@@ -521,9 +521,6 @@
     <t>S7042-ND</t>
   </si>
   <si>
-    <t>895-USB-RS485-PCBA</t>
-  </si>
-  <si>
     <t>R16</t>
   </si>
   <si>
@@ -632,9 +629,6 @@
     <t>296-2061-5-ND</t>
   </si>
   <si>
-    <t>595-CD4066BE</t>
-  </si>
-  <si>
     <t>U2</t>
   </si>
   <si>
@@ -707,7 +701,7 @@
     <t>A32244-ND</t>
   </si>
   <si>
-    <t>571-2212369-1</t>
+    <t>571-2213362-1</t>
   </si>
   <si>
     <t>R20-R26</t>
@@ -749,6 +743,21 @@
     <t>RMCF0805JT1K80CT-ND</t>
   </si>
   <si>
+    <t>XA1</t>
+  </si>
+  <si>
+    <t>Conn_Poncho2P_2x_20x2</t>
+  </si>
+  <si>
+    <t>osc:poncho_grande</t>
+  </si>
+  <si>
+    <t>PEC20DAAN</t>
+  </si>
+  <si>
+    <t>S2012E-20-ND</t>
+  </si>
+  <si>
     <t>U3</t>
   </si>
   <si>
@@ -836,22 +845,7 @@
     <t>296-1781-5-ND</t>
   </si>
   <si>
-    <t>XA1</t>
-  </si>
-  <si>
-    <t>Conn_Poncho2P_2x_20x2</t>
-  </si>
-  <si>
-    <t>osc:poncho_grande</t>
-  </si>
-  <si>
-    <t>PPTC202LFBN-RC</t>
-  </si>
-  <si>
-    <t>S6104-ND</t>
-  </si>
-  <si>
-    <t>517-N2550-6002RB</t>
+    <t>595-TL082IP</t>
   </si>
   <si>
     <t>U1</t>
@@ -867,6 +861,9 @@
   </si>
   <si>
     <t>296-1402-5-ND</t>
+  </si>
+  <si>
+    <t>595-MAX232N</t>
   </si>
   <si>
     <t>RV1</t>
@@ -1174,22 +1171,16 @@
   <dimension ref="A1:AA65"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="9" ySplit="6" topLeftCell="J13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="6" topLeftCell="U10" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="E16" activeCellId="0" sqref="E16"/>
+      <selection pane="topRight" activeCell="U1" activeCellId="0" sqref="U1"/>
+      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1020408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.14285714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.7959183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="38.3622448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.0510204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="9.14285714285714"/>
+    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="9.14285714285714"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.7142857142857"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.14285714285714"/>
     <col collapsed="false" hidden="false" max="12" min="11" style="0" width="9.14285714285714"/>
@@ -1203,7 +1194,7 @@
     <col collapsed="false" hidden="false" max="24" min="23" style="0" width="9.14285714285714"/>
     <col collapsed="false" hidden="false" max="25" min="25" style="0" width="15.7142857142857"/>
     <col collapsed="false" hidden="false" max="27" min="26" style="0" width="9.14285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="8.6734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1211,7 +1202,7 @@
         <v>0</v>
       </c>
       <c r="I1" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1220,15 +1211,15 @@
       </c>
       <c r="I2" s="3" t="n">
         <f aca="false">SUM(I7:I35)</f>
-        <v>96.123</v>
+        <v>20.879</v>
       </c>
       <c r="M2" s="3" t="n">
         <f aca="false">SUM(M7:M35)</f>
-        <v>76.643</v>
+        <v>16.99</v>
       </c>
       <c r="S2" s="3" t="n">
         <f aca="false">SUM(S7:S35)</f>
-        <v>451.14</v>
+        <v>36.439</v>
       </c>
       <c r="Y2" s="3" t="n">
         <f aca="false">SUM(Y7:Y35)</f>
@@ -1241,7 +1232,7 @@
       </c>
       <c r="I3" s="4" t="n">
         <f aca="false">TotalCost/BoardQty</f>
-        <v>19.2246</v>
+        <v>20.879</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1382,26 +1373,26 @@
       </c>
       <c r="G7" s="0" t="n">
         <f aca="false">BoardQty*4</f>
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="H7" s="10" t="n">
         <f aca="true">MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0.17</v>
+        <v>0.21</v>
       </c>
       <c r="I7" s="10" t="n">
         <f aca="false">IFERROR(G7*H7,"")</f>
-        <v>3.4</v>
+        <v>0.84</v>
       </c>
       <c r="J7" s="0" t="n">
         <v>0</v>
       </c>
       <c r="L7" s="10" t="n">
         <f aca="false">IFERROR(LOOKUP(IF(K7="",G7,K7),{0,1,10,100,500,1000},{0,0.21,0.17,0.0898,0.05906,0.04024}),"")</f>
-        <v>0.17</v>
+        <v>0.21</v>
       </c>
       <c r="M7" s="10" t="n">
         <f aca="false">IFERROR(IF(K7="",G7,K7)*L7,"")</f>
-        <v>3.4</v>
+        <v>0.84</v>
       </c>
       <c r="N7" s="0" t="s">
         <v>25</v>
@@ -1425,7 +1416,7 @@
       </c>
       <c r="G8" s="0" t="n">
         <f aca="false">BoardQty*3</f>
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="H8" s="10" t="n">
         <f aca="true">MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
@@ -1454,7 +1445,7 @@
       </c>
       <c r="G9" s="0" t="n">
         <f aca="false">BoardQty*1</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H9" s="10" t="n">
         <f aca="true">MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
@@ -1462,7 +1453,7 @@
       </c>
       <c r="I9" s="10" t="n">
         <f aca="false">IFERROR(G9*H9,"")</f>
-        <v>4.15</v>
+        <v>0.83</v>
       </c>
       <c r="J9" s="0" t="n">
         <v>0</v>
@@ -1473,7 +1464,7 @@
       </c>
       <c r="M9" s="10" t="n">
         <f aca="false">IFERROR(IF(K9="",G9,K9)*L9,"")</f>
-        <v>4.15</v>
+        <v>0.83</v>
       </c>
       <c r="N9" s="0" t="s">
         <v>35</v>
@@ -1481,46 +1472,29 @@
       <c r="O9" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="P9" s="0" t="n">
-        <v>390</v>
-      </c>
-      <c r="R9" s="10" t="n">
-        <f aca="false">IFERROR(LOOKUP(IF(Q9="",G9,Q9),{0,1,10},{0,24.93,24.5}),"")</f>
-        <v>24.93</v>
-      </c>
-      <c r="S9" s="10" t="n">
-        <f aca="false">IFERROR(IF(Q9="",G9,Q9)*R9,"")</f>
-        <v>124.65</v>
-      </c>
-      <c r="T9" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="U9" s="11" t="s">
-        <v>26</v>
-      </c>
       <c r="AA9" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="D10" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="E10" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="F10" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="G10" s="0" t="n">
         <f aca="false">BoardQty*1</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H10" s="10" t="n">
         <f aca="true">MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
@@ -1528,21 +1502,21 @@
       </c>
       <c r="I10" s="10" t="n">
         <f aca="false">IFERROR(G10*H10,"")</f>
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="J10" s="0" t="n">
         <v>0</v>
       </c>
       <c r="L10" s="10" t="n">
-        <f aca="false">IFERROR(LOOKUP(IF(K10="",G10,K10),{0,1,10,50,100,250,500,1000,2500},{0,0.1,0.017,0.0092,0.0067,0.00516,0.00412,0.00303,0.00263}),"")</f>
+        <f aca="false">IFERROR(LOOKUP(IF(K10="",G10,K10),{0,1,10,25,50,100,250,500,1000},{0,0.1,0.015,0.0108,0.0084,0.0061,0.00468,0.00374,0.00276}),"")</f>
         <v>0.1</v>
       </c>
       <c r="M10" s="10" t="n">
         <f aca="false">IFERROR(IF(K10="",G10,K10)*L10,"")</f>
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="N10" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O10" s="11" t="s">
         <v>26</v>
@@ -1550,62 +1524,62 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="D11" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="E11" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="F11" s="0" t="s">
         <v>46</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>47</v>
       </c>
       <c r="G11" s="0" t="n">
         <f aca="false">BoardQty*2</f>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H11" s="10" t="n">
         <f aca="true">MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0.21</v>
+        <v>0.31</v>
       </c>
       <c r="I11" s="10" t="n">
         <f aca="false">IFERROR(G11*H11,"")</f>
-        <v>2.1</v>
+        <v>0.62</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>0</v>
       </c>
       <c r="L11" s="10" t="n">
         <f aca="false">IFERROR(LOOKUP(IF(K11="",G11,K11),{0,1,10,100,500,1000},{0,0.31,0.255,0.135,0.08878,0.06049}),"")</f>
-        <v>0.255</v>
+        <v>0.31</v>
       </c>
       <c r="M11" s="10" t="n">
         <f aca="false">IFERROR(IF(K11="",G11,K11)*L11,"")</f>
-        <v>2.55</v>
+        <v>0.62</v>
       </c>
       <c r="N11" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O11" s="11" t="s">
         <v>26</v>
       </c>
       <c r="P11" s="0" t="n">
-        <v>9862</v>
+        <v>9747</v>
       </c>
       <c r="R11" s="10" t="n">
-        <f aca="false">IFERROR(LOOKUP(IF(Q11="",G11,Q11),{0,1,10,100,1000,2500,10000,20000,50000,100000},{0,0.316,0.21,0.088,0.059,0.046,0.038,0.036,0.034,0.029}),"")</f>
-        <v>0.21</v>
+        <f aca="false">IFERROR(LOOKUP(IF(Q11="",G11,Q11),{0,1,10,100,1000,2500,10000,20000,50000,100000},{0,0.32,0.213,0.089,0.06,0.046,0.039,0.037,0.034,0.031}),"")</f>
+        <v>0.32</v>
       </c>
       <c r="S11" s="10" t="n">
         <f aca="false">IFERROR(IF(Q11="",G11,Q11)*R11,"")</f>
-        <v>2.1</v>
+        <v>0.64</v>
       </c>
       <c r="T11" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="U11" s="11" t="s">
         <v>26</v>
@@ -1613,23 +1587,23 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="0" t="s">
         <v>50</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>51</v>
       </c>
       <c r="G12" s="0" t="n">
         <f aca="false">BoardQty*1</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H12" s="10" t="n">
         <f aca="true">MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
@@ -1637,7 +1611,7 @@
       </c>
       <c r="I12" s="10" t="n">
         <f aca="false">IFERROR(G12*H12,"")</f>
-        <v>1.55</v>
+        <v>0.31</v>
       </c>
       <c r="J12" s="0" t="n">
         <v>0</v>
@@ -1648,27 +1622,27 @@
       </c>
       <c r="M12" s="10" t="n">
         <f aca="false">IFERROR(IF(K12="",G12,K12)*L12,"")</f>
-        <v>1.55</v>
+        <v>0.31</v>
       </c>
       <c r="N12" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O12" s="11" t="s">
         <v>26</v>
       </c>
       <c r="P12" s="0" t="n">
-        <v>9862</v>
+        <v>9747</v>
       </c>
       <c r="R12" s="10" t="n">
-        <f aca="false">IFERROR(LOOKUP(IF(Q12="",G12,Q12),{0,1,10,100,1000,2500,10000,20000,50000,100000},{0,0.316,0.21,0.088,0.059,0.046,0.038,0.036,0.034,0.029}),"")</f>
-        <v>0.316</v>
+        <f aca="false">IFERROR(LOOKUP(IF(Q12="",G12,Q12),{0,1,10,100,1000,2500,10000,20000,50000,100000},{0,0.32,0.213,0.089,0.06,0.046,0.039,0.037,0.034,0.031}),"")</f>
+        <v>0.32</v>
       </c>
       <c r="S12" s="10" t="n">
         <f aca="false">IFERROR(IF(Q12="",G12,Q12)*R12,"")</f>
-        <v>1.58</v>
+        <v>0.32</v>
       </c>
       <c r="T12" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="U12" s="11" t="s">
         <v>26</v>
@@ -1676,45 +1650,45 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="D13" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="0" t="s">
         <v>53</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>54</v>
       </c>
       <c r="G13" s="0" t="n">
         <f aca="false">BoardQty*5</f>
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="H13" s="10" t="n">
         <f aca="true">MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0.017</v>
+        <v>0.1</v>
       </c>
       <c r="I13" s="10" t="n">
         <f aca="false">IFERROR(G13*H13,"")</f>
-        <v>0.425</v>
+        <v>0.5</v>
       </c>
       <c r="J13" s="0" t="n">
         <v>0</v>
       </c>
       <c r="L13" s="10" t="n">
-        <f aca="false">IFERROR(LOOKUP(IF(K13="",G13,K13),{0,1,10,50,100,250,500,1000,2500},{0,0.1,0.017,0.0092,0.0067,0.00516,0.00412,0.00303,0.00263}),"")</f>
-        <v>0.017</v>
+        <f aca="false">IFERROR(LOOKUP(IF(K13="",G13,K13),{0,1,10,25,50,100,250,500,1000},{0,0.1,0.015,0.0108,0.0084,0.0061,0.00468,0.00374,0.00276}),"")</f>
+        <v>0.1</v>
       </c>
       <c r="M13" s="10" t="n">
         <f aca="false">IFERROR(IF(K13="",G13,K13)*L13,"")</f>
-        <v>0.425</v>
+        <v>0.5</v>
       </c>
       <c r="N13" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O13" s="11" t="s">
         <v>26</v>
@@ -1722,23 +1696,23 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="D14" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>58</v>
-      </c>
       <c r="F14" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G14" s="0" t="n">
         <f aca="false">BoardQty*1</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H14" s="10" t="n">
         <f aca="true">MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
@@ -1746,7 +1720,7 @@
       </c>
       <c r="I14" s="10" t="n">
         <f aca="false">IFERROR(G14*H14,"")</f>
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="J14" s="0" t="n">
         <v>0</v>
@@ -1757,10 +1731,10 @@
       </c>
       <c r="M14" s="10" t="n">
         <f aca="false">IFERROR(IF(K14="",G14,K14)*L14,"")</f>
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="N14" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O14" s="11" t="s">
         <v>26</v>
@@ -1769,15 +1743,15 @@
         <v>39</v>
       </c>
       <c r="R14" s="10" t="n">
-        <f aca="false">IFERROR(LOOKUP(IF(Q14="",G14,Q14),{0,1,10,25,50,100,250,500,1000,2500},{0,9.42,8.47,7.72,7.18,6.97,6.37,5.8,4.92,4.77}),"")</f>
-        <v>9.42</v>
+        <f aca="false">IFERROR(LOOKUP(IF(Q14="",G14,Q14),{0,1,10,25,50,100,250,500,1000,2500},{0,9.44,8.5,7.74,7.21,6.99,6.38,5.82,4.93,4.91}),"")</f>
+        <v>9.44</v>
       </c>
       <c r="S14" s="10" t="n">
         <f aca="false">IFERROR(IF(Q14="",G14,Q14)*R14,"")</f>
-        <v>47.1</v>
+        <v>9.44</v>
       </c>
       <c r="T14" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="U14" s="11" t="s">
         <v>26</v>
@@ -1785,23 +1759,23 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="0" t="s">
         <v>61</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>62</v>
       </c>
       <c r="G15" s="0" t="n">
         <f aca="false">BoardQty*1</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H15" s="10" t="n">
         <f aca="true">MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
@@ -1809,7 +1783,7 @@
       </c>
       <c r="I15" s="10" t="n">
         <f aca="false">IFERROR(G15*H15,"")</f>
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="J15" s="0" t="n">
         <v>0</v>
@@ -1820,34 +1794,51 @@
       </c>
       <c r="M15" s="10" t="n">
         <f aca="false">IFERROR(IF(K15="",G15,K15)*L15,"")</f>
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="N15" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="O15" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="P15" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="R15" s="10" t="n">
+        <f aca="false">IFERROR(LOOKUP(IF(Q15="",G15,Q15),{0,1,10,25,50,100,250,500,1000,2500},{0,9.44,8.5,7.74,7.21,6.99,6.38,5.82,4.93,4.91}),"")</f>
+        <v>9.44</v>
+      </c>
+      <c r="S15" s="10" t="n">
+        <f aca="false">IFERROR(IF(Q15="",G15,Q15)*R15,"")</f>
+        <v>9.44</v>
+      </c>
+      <c r="T15" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="O15" s="11" t="s">
+      <c r="U15" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="D16" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="0" t="s">
         <v>64</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>65</v>
       </c>
       <c r="G16" s="0" t="n">
         <f aca="false">BoardQty*1</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H16" s="10" t="n">
         <f aca="true">MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
@@ -1855,21 +1846,21 @@
       </c>
       <c r="I16" s="10" t="n">
         <f aca="false">IFERROR(G16*H16,"")</f>
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="J16" s="0" t="n">
         <v>0</v>
       </c>
       <c r="L16" s="10" t="n">
-        <f aca="false">IFERROR(LOOKUP(IF(K16="",G16,K16),{0,1,10,50,100,250,500,1000,2500},{0,0.1,0.017,0.0092,0.0067,0.00516,0.00412,0.00303,0.00263}),"")</f>
+        <f aca="false">IFERROR(LOOKUP(IF(K16="",G16,K16),{0,1,10,25,50,100,250,500,1000},{0,0.1,0.015,0.0108,0.0084,0.0061,0.00468,0.00374,0.00276}),"")</f>
         <v>0.1</v>
       </c>
       <c r="M16" s="10" t="n">
         <f aca="false">IFERROR(IF(K16="",G16,K16)*L16,"")</f>
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="N16" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O16" s="11" t="s">
         <v>26</v>
@@ -1877,31 +1868,31 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="D17" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="E17" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="F17" s="0" t="s">
         <v>70</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>71</v>
       </c>
       <c r="G17" s="0" t="n">
         <f aca="false">BoardQty*1</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H17" s="10" t="n">
         <f aca="true">MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0.463</v>
+        <v>0.48</v>
       </c>
       <c r="I17" s="10" t="n">
         <f aca="false">IFERROR(G17*H17,"")</f>
-        <v>2.315</v>
+        <v>0.48</v>
       </c>
       <c r="J17" s="0" t="n">
         <v>0</v>
@@ -1912,29 +1903,12 @@
       </c>
       <c r="M17" s="10" t="n">
         <f aca="false">IFERROR(IF(K17="",G17,K17)*L17,"")</f>
-        <v>2.4</v>
+        <v>0.48</v>
       </c>
       <c r="N17" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O17" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="P17" s="0" t="n">
-        <v>9494</v>
-      </c>
-      <c r="R17" s="10" t="n">
-        <f aca="false">IFERROR(LOOKUP(IF(Q17="",G17,Q17),{0,1,10,100,1000,2500,10000,25000},{0,0.463,0.391,0.239,0.184,0.158,0.146,0.138}),"")</f>
-        <v>0.463</v>
-      </c>
-      <c r="S17" s="10" t="n">
-        <f aca="false">IFERROR(IF(Q17="",G17,Q17)*R17,"")</f>
-        <v>2.315</v>
-      </c>
-      <c r="T17" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="U17" s="11" t="s">
         <v>26</v>
       </c>
       <c r="AA17" s="11" t="s">
@@ -1943,23 +1917,23 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>22</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G18" s="0" t="n">
         <f aca="false">BoardQty*1</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H18" s="10" t="n">
         <f aca="true">MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
@@ -1967,7 +1941,7 @@
       </c>
       <c r="I18" s="10" t="n">
         <f aca="false">IFERROR(G18*H18,"")</f>
-        <v>2.5</v>
+        <v>0.5</v>
       </c>
       <c r="J18" s="0" t="n">
         <v>0</v>
@@ -1978,10 +1952,10 @@
       </c>
       <c r="M18" s="10" t="n">
         <f aca="false">IFERROR(IF(K18="",G18,K18)*L18,"")</f>
-        <v>2.5</v>
+        <v>0.5</v>
       </c>
       <c r="N18" s="0" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="O18" s="11" t="s">
         <v>26</v>
@@ -1992,45 +1966,45 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="E19" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="F19" s="0" t="s">
         <v>80</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>82</v>
       </c>
       <c r="G19" s="0" t="n">
         <f aca="false">BoardQty*8</f>
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="H19" s="10" t="n">
         <f aca="true">MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0.0132</v>
+        <v>0.1</v>
       </c>
       <c r="I19" s="10" t="n">
         <f aca="false">IFERROR(G19*H19,"")</f>
-        <v>0.528</v>
+        <v>0.8</v>
       </c>
       <c r="J19" s="0" t="n">
         <v>0</v>
       </c>
       <c r="L19" s="10" t="n">
         <f aca="false">IFERROR(LOOKUP(IF(K19="",G19,K19),{0,1,10,25,50,100,250,500,1000},{0,0.1,0.018,0.0132,0.01,0.0081,0.00676,0.00578,0.00454}),"")</f>
-        <v>0.0132</v>
+        <v>0.1</v>
       </c>
       <c r="M19" s="10" t="n">
         <f aca="false">IFERROR(IF(K19="",G19,K19)*L19,"")</f>
-        <v>0.528</v>
+        <v>0.8</v>
       </c>
       <c r="N19" s="0" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="O19" s="11" t="s">
         <v>26</v>
@@ -2038,23 +2012,23 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="0" t="s">
         <v>84</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>86</v>
       </c>
       <c r="G20" s="0" t="n">
         <f aca="false">BoardQty*1</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H20" s="10" t="n">
         <f aca="true">MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
@@ -2062,21 +2036,21 @@
       </c>
       <c r="I20" s="10" t="n">
         <f aca="false">IFERROR(G20*H20,"")</f>
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="J20" s="0" t="n">
         <v>0</v>
       </c>
       <c r="L20" s="10" t="n">
-        <f aca="false">IFERROR(LOOKUP(IF(K20="",G20,K20),{0,1,10,50,100,250,500,1000,2500,5000},{0,0.1,0.018,0.0096,0.0071,0.00544,0.00436,0.00321,0.00278,0.0023}),"")</f>
+        <f aca="false">IFERROR(LOOKUP(IF(K20="",G20,K20),{0,1,10,25,50,100,250,500,1000,5000},{0,0.1,0.016,0.0116,0.0088,0.0065,0.00496,0.00396,0.00292,0.00209}),"")</f>
         <v>0.1</v>
       </c>
       <c r="M20" s="10" t="n">
         <f aca="false">IFERROR(IF(K20="",G20,K20)*L20,"")</f>
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="N20" s="0" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="O20" s="11" t="s">
         <v>26</v>
@@ -2084,45 +2058,45 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="0" t="s">
         <v>88</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>90</v>
       </c>
       <c r="G21" s="0" t="n">
         <f aca="false">BoardQty*3</f>
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="H21" s="10" t="n">
         <f aca="true">MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0.017</v>
+        <v>0.1</v>
       </c>
       <c r="I21" s="10" t="n">
         <f aca="false">IFERROR(G21*H21,"")</f>
-        <v>0.255</v>
+        <v>0.3</v>
       </c>
       <c r="J21" s="0" t="n">
         <v>0</v>
       </c>
       <c r="L21" s="10" t="n">
-        <f aca="false">IFERROR(LOOKUP(IF(K21="",G21,K21),{0,1,10,50,100,250,500,1000,2500},{0,0.1,0.017,0.0092,0.0067,0.00516,0.00412,0.00303,0.00263}),"")</f>
-        <v>0.017</v>
+        <f aca="false">IFERROR(LOOKUP(IF(K21="",G21,K21),{0,1,10,25,50,100,250,500,1000},{0,0.1,0.015,0.0108,0.0084,0.0061,0.00468,0.00374,0.00276}),"")</f>
+        <v>0.1</v>
       </c>
       <c r="M21" s="10" t="n">
         <f aca="false">IFERROR(IF(K21="",G21,K21)*L21,"")</f>
-        <v>0.255</v>
+        <v>0.3</v>
       </c>
       <c r="N21" s="0" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="O21" s="11" t="s">
         <v>26</v>
@@ -2130,23 +2104,23 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="E22" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="F22" s="0" t="s">
         <v>94</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="F22" s="0" t="s">
-        <v>96</v>
       </c>
       <c r="G22" s="0" t="n">
         <f aca="false">BoardQty*1</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H22" s="10" t="n">
         <f aca="true">MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
@@ -2154,7 +2128,7 @@
       </c>
       <c r="I22" s="10" t="n">
         <f aca="false">IFERROR(G22*H22,"")</f>
-        <v>17.05</v>
+        <v>3.41</v>
       </c>
       <c r="J22" s="0" t="n">
         <v>0</v>
@@ -2165,27 +2139,27 @@
       </c>
       <c r="M22" s="10" t="n">
         <f aca="false">IFERROR(IF(K22="",G22,K22)*L22,"")</f>
-        <v>17.05</v>
+        <v>3.41</v>
       </c>
       <c r="N22" s="0" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O22" s="11" t="s">
         <v>26</v>
       </c>
       <c r="P22" s="0" t="n">
-        <v>66</v>
+        <v>4870</v>
       </c>
       <c r="R22" s="10" t="n">
-        <f aca="false">IFERROR(LOOKUP(IF(Q22="",G22,Q22),{0,1,5,10,25,50,100},{0,47.47,46.44,42.72,39.23,38.13,32.04}),"")</f>
-        <v>46.44</v>
+        <f aca="false">IFERROR(LOOKUP(IF(Q22="",G22,Q22),{0,1,10,20,50,100,200,500,1000},{0,10.07,9.22,8.95,8.38,8.11,7.82,7.44,7.27}),"")</f>
+        <v>10.07</v>
       </c>
       <c r="S22" s="10" t="n">
         <f aca="false">IFERROR(IF(Q22="",G22,Q22)*R22,"")</f>
-        <v>232.2</v>
+        <v>10.07</v>
       </c>
       <c r="T22" s="0" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="U22" s="11" t="s">
         <v>26</v>
@@ -2196,45 +2170,45 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="0" t="s">
         <v>99</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="F23" s="0" t="s">
-        <v>101</v>
       </c>
       <c r="G23" s="0" t="n">
         <f aca="false">BoardQty*7</f>
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="H23" s="10" t="n">
         <f aca="true">MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0.017</v>
+        <v>0.1</v>
       </c>
       <c r="I23" s="10" t="n">
         <f aca="false">IFERROR(G23*H23,"")</f>
-        <v>0.595</v>
+        <v>0.7</v>
       </c>
       <c r="J23" s="0" t="n">
         <v>0</v>
       </c>
       <c r="L23" s="10" t="n">
-        <f aca="false">IFERROR(LOOKUP(IF(K23="",G23,K23),{0,1,10,50,100,250,500,1000,2500},{0,0.1,0.017,0.0092,0.0067,0.00516,0.00412,0.00303,0.00263}),"")</f>
-        <v>0.017</v>
+        <f aca="false">IFERROR(LOOKUP(IF(K23="",G23,K23),{0,1,10,25,50,100,250,500,1000},{0,0.1,0.015,0.0108,0.0084,0.0061,0.00468,0.00374,0.00276}),"")</f>
+        <v>0.1</v>
       </c>
       <c r="M23" s="10" t="n">
         <f aca="false">IFERROR(IF(K23="",G23,K23)*L23,"")</f>
-        <v>0.595</v>
+        <v>0.7</v>
       </c>
       <c r="N23" s="0" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="O23" s="11" t="s">
         <v>26</v>
@@ -2242,23 +2216,23 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="E24" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="B24" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="0" t="s">
+      <c r="F24" s="0" t="s">
         <v>104</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="F24" s="0" t="s">
-        <v>106</v>
       </c>
       <c r="G24" s="0" t="n">
         <f aca="false">BoardQty*1</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H24" s="10" t="n">
         <f aca="true">MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
@@ -2266,21 +2240,21 @@
       </c>
       <c r="I24" s="10" t="n">
         <f aca="false">IFERROR(G24*H24,"")</f>
-        <v>7.5</v>
+        <v>1.5</v>
       </c>
       <c r="J24" s="0" t="n">
         <v>0</v>
       </c>
       <c r="L24" s="10" t="n">
-        <f aca="false">IFERROR(LOOKUP(IF(K24="",G24,K24),{0,1,10,25,50,100,250,500,1000,2500},{0,1.5,1.32,1.188,1.144,1.1,1.034,0.88,0.814,0.704}),"")</f>
+        <f aca="false">IFERROR(LOOKUP(IF(K24="",G24,K24),{0,1,10,25,50,100,250,500,1000,5000},{0,1.5,1.32,1.188,1.144,1.1,1.034,0.88,0.814,0.6688}),"")</f>
         <v>1.5</v>
       </c>
       <c r="M24" s="10" t="n">
         <f aca="false">IFERROR(IF(K24="",G24,K24)*L24,"")</f>
-        <v>7.5</v>
+        <v>1.5</v>
       </c>
       <c r="N24" s="0" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="O24" s="11" t="s">
         <v>26</v>
@@ -2288,23 +2262,23 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F25" s="0" t="s">
         <v>108</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="F25" s="0" t="s">
-        <v>110</v>
       </c>
       <c r="G25" s="0" t="n">
         <f aca="false">BoardQty*1</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H25" s="10" t="n">
         <f aca="true">MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
@@ -2312,21 +2286,21 @@
       </c>
       <c r="I25" s="10" t="n">
         <f aca="false">IFERROR(G25*H25,"")</f>
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="J25" s="0" t="n">
         <v>0</v>
       </c>
       <c r="L25" s="10" t="n">
-        <f aca="false">IFERROR(LOOKUP(IF(K25="",G25,K25),{0,1,10,50,100,250,500,1000,2500},{0,0.1,0.017,0.0092,0.0067,0.00516,0.00412,0.00303,0.00263}),"")</f>
+        <f aca="false">IFERROR(LOOKUP(IF(K25="",G25,K25),{0,1,10,25,50,100,250,500,1000},{0,0.1,0.015,0.0108,0.0084,0.0061,0.00468,0.00374,0.00276}),"")</f>
         <v>0.1</v>
       </c>
       <c r="M25" s="10" t="n">
         <f aca="false">IFERROR(IF(K25="",G25,K25)*L25,"")</f>
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="N25" s="0" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O25" s="11" t="s">
         <v>26</v>
@@ -2334,64 +2308,47 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="D26" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="E26" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" s="0" t="s">
         <v>113</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="F26" s="0" t="s">
-        <v>114</v>
       </c>
       <c r="G26" s="0" t="n">
         <f aca="false">BoardQty*1</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H26" s="10" t="n">
         <f aca="true">MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0.453</v>
+        <v>1.82</v>
       </c>
       <c r="I26" s="10" t="n">
         <f aca="false">IFERROR(G26*H26,"")</f>
-        <v>2.265</v>
+        <v>1.82</v>
       </c>
       <c r="J26" s="0" t="n">
         <v>0</v>
       </c>
       <c r="L26" s="10" t="n">
-        <f aca="false">IFERROR(LOOKUP(IF(K26="",G26,K26),{0,1,10,100,500,1000},{0,0.48,0.387,0.264,0.1976,0.148}),"")</f>
-        <v>0.48</v>
+        <f aca="false">IFERROR(LOOKUP(IF(K26="",G26,K26),{0,1,10,100,500,1000,5000,10000},{0,1.82,1.632,1.344,1.0624,0.912,0.832,0.8}),"")</f>
+        <v>1.82</v>
       </c>
       <c r="M26" s="10" t="n">
         <f aca="false">IFERROR(IF(K26="",G26,K26)*L26,"")</f>
-        <v>2.4</v>
+        <v>1.82</v>
       </c>
       <c r="N26" s="0" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="O26" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="P26" s="0" t="n">
-        <v>2777</v>
-      </c>
-      <c r="R26" s="10" t="n">
-        <f aca="false">IFERROR(LOOKUP(IF(Q26="",G26,Q26),{0,1,10,100,1000,2000,10000,24000,50000},{0,0.453,0.349,0.19,0.142,0.122,0.113,0.105,0.1}),"")</f>
-        <v>0.453</v>
-      </c>
-      <c r="S26" s="10" t="n">
-        <f aca="false">IFERROR(IF(Q26="",G26,Q26)*R26,"")</f>
-        <v>2.265</v>
-      </c>
-      <c r="T26" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="U26" s="11" t="s">
         <v>26</v>
       </c>
       <c r="AA26" s="11" t="s">
@@ -2400,69 +2357,86 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="B27" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="F27" s="0" t="s">
-        <v>119</v>
-      </c>
       <c r="G27" s="0" t="n">
-        <f aca="false">BoardQty*4</f>
-        <v>20</v>
+        <f aca="false">BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="H27" s="10" t="n">
         <f aca="true">MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0.017</v>
+        <v>0.46</v>
       </c>
       <c r="I27" s="10" t="n">
         <f aca="false">IFERROR(G27*H27,"")</f>
-        <v>0.34</v>
+        <v>0.46</v>
       </c>
       <c r="J27" s="0" t="n">
         <v>0</v>
       </c>
       <c r="L27" s="10" t="n">
-        <f aca="false">IFERROR(LOOKUP(IF(K27="",G27,K27),{0,1,10,50,100,250,500,1000,2500},{0,0.1,0.017,0.0092,0.0067,0.00516,0.00412,0.00303,0.00263}),"")</f>
-        <v>0.017</v>
+        <f aca="false">IFERROR(LOOKUP(IF(K27="",G27,K27),{0,1,10,100,500,1000},{0,0.48,0.387,0.264,0.1976,0.148}),"")</f>
+        <v>0.48</v>
       </c>
       <c r="M27" s="10" t="n">
         <f aca="false">IFERROR(IF(K27="",G27,K27)*L27,"")</f>
-        <v>0.34</v>
+        <v>0.48</v>
       </c>
       <c r="N27" s="0" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="O27" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="P27" s="0" t="n">
+        <v>2773</v>
+      </c>
+      <c r="R27" s="10" t="n">
+        <f aca="false">IFERROR(LOOKUP(IF(Q27="",G27,Q27),{0,1,10,100,1000,2000,10000,24000,50000},{0,0.46,0.354,0.192,0.144,0.124,0.114,0.106,0.104}),"")</f>
+        <v>0.46</v>
+      </c>
+      <c r="S27" s="10" t="n">
+        <f aca="false">IFERROR(IF(Q27="",G27,Q27)*R27,"")</f>
+        <v>0.46</v>
+      </c>
+      <c r="T27" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="U27" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B28" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="D28" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F28" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="D28" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="F28" s="0" t="s">
-        <v>123</v>
-      </c>
       <c r="G28" s="0" t="n">
-        <f aca="false">BoardQty*1</f>
-        <v>5</v>
+        <f aca="false">BoardQty*4</f>
+        <v>4</v>
       </c>
       <c r="H28" s="10" t="n">
         <f aca="true">MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
@@ -2470,21 +2444,21 @@
       </c>
       <c r="I28" s="10" t="n">
         <f aca="false">IFERROR(G28*H28,"")</f>
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J28" s="0" t="n">
         <v>0</v>
       </c>
       <c r="L28" s="10" t="n">
-        <f aca="false">IFERROR(LOOKUP(IF(K28="",G28,K28),{0,1,10,50,100,250,500,1000,2500},{0,0.1,0.017,0.0092,0.0067,0.00516,0.00412,0.00303,0.00263}),"")</f>
+        <f aca="false">IFERROR(LOOKUP(IF(K28="",G28,K28),{0,1,10,25,50,100,250,500,1000},{0,0.1,0.015,0.0108,0.0084,0.0061,0.00468,0.00374,0.00276}),"")</f>
         <v>0.1</v>
       </c>
       <c r="M28" s="10" t="n">
         <f aca="false">IFERROR(IF(K28="",G28,K28)*L28,"")</f>
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="O28" s="11" t="s">
         <v>26</v>
@@ -2492,23 +2466,23 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B29" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="D29" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F29" s="0" t="s">
         <v>126</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="F29" s="0" t="s">
-        <v>127</v>
       </c>
       <c r="G29" s="0" t="n">
         <f aca="false">BoardQty*1</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H29" s="10" t="n">
         <f aca="true">MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
@@ -2516,21 +2490,21 @@
       </c>
       <c r="I29" s="10" t="n">
         <f aca="false">IFERROR(G29*H29,"")</f>
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="J29" s="0" t="n">
         <v>0</v>
       </c>
       <c r="L29" s="10" t="n">
-        <f aca="false">IFERROR(LOOKUP(IF(K29="",G29,K29),{0,1,10,50,100,250,500,1000,2500},{0,0.1,0.017,0.0092,0.0067,0.00516,0.00412,0.00303,0.00263}),"")</f>
+        <f aca="false">IFERROR(LOOKUP(IF(K29="",G29,K29),{0,1,10,25,50,100,250,500,1000},{0,0.1,0.015,0.0108,0.0084,0.0061,0.00468,0.00374,0.00276}),"")</f>
         <v>0.1</v>
       </c>
       <c r="M29" s="10" t="n">
         <f aca="false">IFERROR(IF(K29="",G29,K29)*L29,"")</f>
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O29" s="11" t="s">
         <v>26</v>
@@ -2538,220 +2512,217 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="B30" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="B30" s="0" t="s">
-        <v>44</v>
-      </c>
       <c r="D30" s="0" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>47</v>
+        <v>130</v>
       </c>
       <c r="G30" s="0" t="n">
         <f aca="false">BoardQty*1</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H30" s="10" t="n">
         <f aca="true">MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0.31</v>
+        <v>0.1</v>
       </c>
       <c r="I30" s="10" t="n">
         <f aca="false">IFERROR(G30*H30,"")</f>
-        <v>1.55</v>
+        <v>0.1</v>
       </c>
       <c r="J30" s="0" t="n">
         <v>0</v>
       </c>
       <c r="L30" s="10" t="n">
-        <f aca="false">IFERROR(LOOKUP(IF(K30="",G30,K30),{0,1,10,100,500,1000},{0,0.31,0.255,0.135,0.08878,0.06049}),"")</f>
-        <v>0.31</v>
+        <f aca="false">IFERROR(LOOKUP(IF(K30="",G30,K30),{0,1,10,25,50,100,250,500,1000},{0,0.1,0.015,0.0108,0.0084,0.0061,0.00468,0.00374,0.00276}),"")</f>
+        <v>0.1</v>
       </c>
       <c r="M30" s="10" t="n">
         <f aca="false">IFERROR(IF(K30="",G30,K30)*L30,"")</f>
-        <v>1.55</v>
+        <v>0.1</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>48</v>
+        <v>131</v>
       </c>
       <c r="O30" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="P30" s="0" t="n">
-        <v>9862</v>
-      </c>
-      <c r="R30" s="10" t="n">
-        <f aca="false">IFERROR(LOOKUP(IF(Q30="",G30,Q30),{0,1,10,100,1000,2500,10000,20000,50000,100000},{0,0.316,0.21,0.088,0.059,0.046,0.038,0.036,0.034,0.029}),"")</f>
-        <v>0.316</v>
-      </c>
-      <c r="S30" s="10" t="n">
-        <f aca="false">IFERROR(IF(Q30="",G30,Q30)*R30,"")</f>
-        <v>1.58</v>
-      </c>
-      <c r="T30" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="U30" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>131</v>
+        <v>43</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>132</v>
+        <v>44</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>133</v>
+        <v>45</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>134</v>
+        <v>46</v>
       </c>
       <c r="G31" s="0" t="n">
-        <f aca="false">BoardQty*5</f>
-        <v>25</v>
+        <f aca="false">BoardQty*1</f>
+        <v>1</v>
       </c>
       <c r="H31" s="10" t="n">
         <f aca="true">MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0.11</v>
+        <v>0.31</v>
       </c>
       <c r="I31" s="10" t="n">
         <f aca="false">IFERROR(G31*H31,"")</f>
-        <v>2.75</v>
+        <v>0.31</v>
       </c>
       <c r="J31" s="0" t="n">
         <v>0</v>
       </c>
       <c r="L31" s="10" t="n">
-        <f aca="false">IFERROR(LOOKUP(IF(K31="",G31,K31),{0,1,50,100,250,500,1000},{0,0.11,0.0894,0.0777,0.06904,0.06064,0.05775}),"")</f>
-        <v>0.11</v>
+        <f aca="false">IFERROR(LOOKUP(IF(K31="",G31,K31),{0,1,10,100,500,1000},{0,0.31,0.255,0.135,0.08878,0.06049}),"")</f>
+        <v>0.31</v>
       </c>
       <c r="M31" s="10" t="n">
         <f aca="false">IFERROR(IF(K31="",G31,K31)*L31,"")</f>
-        <v>2.75</v>
+        <v>0.31</v>
       </c>
       <c r="N31" s="0" t="s">
-        <v>135</v>
+        <v>47</v>
       </c>
       <c r="O31" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="P31" s="0" t="n">
+        <v>9747</v>
+      </c>
+      <c r="R31" s="10" t="n">
+        <f aca="false">IFERROR(LOOKUP(IF(Q31="",G31,Q31),{0,1,10,100,1000,2500,10000,20000,50000,100000},{0,0.32,0.213,0.089,0.06,0.046,0.039,0.037,0.034,0.031}),"")</f>
+        <v>0.32</v>
+      </c>
+      <c r="S31" s="10" t="n">
+        <f aca="false">IFERROR(IF(Q31="",G31,Q31)*R31,"")</f>
+        <v>0.32</v>
+      </c>
+      <c r="T31" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="U31" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="E32" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="F32" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="D32" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="F32" s="0" t="s">
-        <v>139</v>
-      </c>
       <c r="G32" s="0" t="n">
-        <f aca="false">BoardQty*1</f>
+        <f aca="false">BoardQty*5</f>
         <v>5</v>
       </c>
       <c r="H32" s="10" t="n">
         <f aca="true">MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0.72</v>
+        <v>0.11</v>
       </c>
       <c r="I32" s="10" t="n">
         <f aca="false">IFERROR(G32*H32,"")</f>
-        <v>3.6</v>
+        <v>0.55</v>
       </c>
       <c r="J32" s="0" t="n">
         <v>0</v>
       </c>
       <c r="L32" s="10" t="n">
-        <f aca="false">IFERROR(LOOKUP(IF(K32="",G32,K32),{0,1,10,100,500,1000,2500,5000,10000},{0,0.72,0.634,0.4858,0.384,0.3072,0.2784,0.2592,0.2496}),"")</f>
-        <v>0.72</v>
+        <f aca="false">IFERROR(LOOKUP(IF(K32="",G32,K32),{0,1,50,100,250,500,1000},{0,0.11,0.0892,0.0778,0.06912,0.06048,0.05761}),"")</f>
+        <v>0.11</v>
       </c>
       <c r="M32" s="10" t="n">
         <f aca="false">IFERROR(IF(K32="",G32,K32)*L32,"")</f>
-        <v>3.6</v>
+        <v>0.55</v>
       </c>
       <c r="N32" s="0" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="O32" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA32" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="D33" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="E33" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F33" s="0" t="s">
         <v>142</v>
-      </c>
-      <c r="D33" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="E33" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="F33" s="0" t="s">
-        <v>144</v>
       </c>
       <c r="G33" s="0" t="n">
         <f aca="false">BoardQty*1</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H33" s="10" t="n">
         <f aca="true">MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>2.73</v>
+        <v>0.749</v>
       </c>
       <c r="I33" s="10" t="n">
         <f aca="false">IFERROR(G33*H33,"")</f>
-        <v>13.65</v>
+        <v>0.749</v>
       </c>
       <c r="J33" s="0" t="n">
         <v>0</v>
       </c>
       <c r="L33" s="10" t="n">
-        <f aca="false">IFERROR(LOOKUP(IF(K33="",G33,K33),{0,1,10,25,50,100,250,500,1000,2500},{0,2.73,2.258,2.1172,1.882,1.6938,1.56208,1.4115,1.25153,1.19978}),"")</f>
-        <v>2.73</v>
+        <f aca="false">IFERROR(LOOKUP(IF(K33="",G33,K33),{0,1,10,100,500,1000,2500,5000,10000},{0,0.75,0.663,0.5085,0.402,0.3216,0.29145,0.27135,0.2613}),"")</f>
+        <v>0.75</v>
       </c>
       <c r="M33" s="10" t="n">
         <f aca="false">IFERROR(IF(K33="",G33,K33)*L33,"")</f>
-        <v>13.65</v>
+        <v>0.75</v>
       </c>
       <c r="N33" s="0" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="O33" s="11" t="s">
         <v>26</v>
       </c>
       <c r="P33" s="0" t="n">
-        <v>3859</v>
+        <v>0</v>
       </c>
       <c r="R33" s="10" t="n">
-        <f aca="false">IFERROR(LOOKUP(IF(Q33="",G33,Q33),{0,1,25,50,100,200,500,1000,2000},{0,3.44,3.01,2.87,2.51,2.44,2.08,1.94,1.86}),"")</f>
-        <v>3.44</v>
+        <f aca="false">IFERROR(LOOKUP(IF(Q33="",G33,Q33),{0,1,10,100,1000,2000,5000,10000},{0,0.749,0.622,0.402,0.322,0.271,0.27,0.262}),"")</f>
+        <v>0.749</v>
       </c>
       <c r="S33" s="10" t="n">
         <f aca="false">IFERROR(IF(Q33="",G33,Q33)*R33,"")</f>
-        <v>17.2</v>
+        <v>0.749</v>
       </c>
       <c r="T33" s="0" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="U33" s="11" t="s">
         <v>26</v>
@@ -2762,31 +2733,31 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="D34" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="E34" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F34" s="0" t="s">
         <v>148</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="E34" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="F34" s="0" t="s">
-        <v>150</v>
       </c>
       <c r="G34" s="0" t="n">
         <f aca="false">BoardQty*1</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H34" s="10" t="n">
         <f aca="true">MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>1.09</v>
+        <v>1.08</v>
       </c>
       <c r="I34" s="10" t="n">
         <f aca="false">IFERROR(G34*H34,"")</f>
-        <v>5.45</v>
+        <v>1.08</v>
       </c>
       <c r="J34" s="0" t="n">
         <v>0</v>
@@ -2797,12 +2768,29 @@
       </c>
       <c r="M34" s="10" t="n">
         <f aca="false">IFERROR(IF(K34="",G34,K34)*L34,"")</f>
-        <v>5.45</v>
+        <v>1.09</v>
       </c>
       <c r="N34" s="0" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="O34" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="P34" s="0" t="n">
+        <v>2817</v>
+      </c>
+      <c r="R34" s="10" t="n">
+        <f aca="false">IFERROR(LOOKUP(IF(Q34="",G34,Q34),{0,1,10,100,500,1000,2500,10000},{0,1.08,0.923,0.71,0.626,0.495,0.437,0.428}),"")</f>
+        <v>1.08</v>
+      </c>
+      <c r="S34" s="10" t="n">
+        <f aca="false">IFERROR(IF(Q34="",G34,Q34)*R34,"")</f>
+        <v>1.08</v>
+      </c>
+      <c r="T34" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="U34" s="11" t="s">
         <v>26</v>
       </c>
       <c r="AA34" s="11" t="s">
@@ -2811,45 +2799,45 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D35" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="B35" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="D35" s="0" t="s">
+      <c r="E35" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="E35" s="0" t="s">
+      <c r="F35" s="0" t="s">
         <v>154</v>
-      </c>
-      <c r="F35" s="0" t="s">
-        <v>155</v>
       </c>
       <c r="G35" s="0" t="n">
         <f aca="false">BoardQty*1</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H35" s="10" t="n">
         <f aca="true">MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>4.03</v>
+        <v>3.92</v>
       </c>
       <c r="I35" s="10" t="n">
         <f aca="false">IFERROR(G35*H35,"")</f>
-        <v>20.15</v>
+        <v>3.92</v>
       </c>
       <c r="P35" s="0" t="n">
-        <v>0</v>
+        <v>465</v>
       </c>
       <c r="R35" s="10" t="n">
-        <f aca="false">IFERROR(LOOKUP(IF(Q35="",G35,Q35),{0,1,25,50,100,500,1000},{0,4.03,3.71,3.37,2.68,2.08,2.02}),"")</f>
-        <v>4.03</v>
+        <f aca="false">IFERROR(LOOKUP(IF(Q35="",G35,Q35),{0,1,25,50,100,500,1000},{0,3.92,3.6,3.28,2.61,2.02,1.96}),"")</f>
+        <v>3.92</v>
       </c>
       <c r="S35" s="10" t="n">
         <f aca="false">IFERROR(IF(Q35="",G35,Q35)*R35,"")</f>
-        <v>20.15</v>
+        <v>3.92</v>
       </c>
       <c r="T35" s="0" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="U35" s="11" t="s">
         <v>26</v>
@@ -4249,9 +4237,9 @@
       <formula>H14</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R17">
+  <conditionalFormatting sqref="R15">
     <cfRule type="cellIs" priority="59" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>H17</formula>
+      <formula>H15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R22">
@@ -4259,14 +4247,14 @@
       <formula>H22</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R26">
+  <conditionalFormatting sqref="R27">
     <cfRule type="cellIs" priority="61" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>H26</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R30">
+      <formula>H27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R31">
     <cfRule type="cellIs" priority="62" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>H30</formula>
+      <formula>H31</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R33">
@@ -4274,14 +4262,14 @@
       <formula>H33</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="R34">
+    <cfRule type="cellIs" priority="64" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>H34</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="R35">
-    <cfRule type="cellIs" priority="64" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="65" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>H35</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R9">
-    <cfRule type="cellIs" priority="65" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>H9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S11">
@@ -4299,9 +4287,9 @@
       <formula>I14</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S17">
+  <conditionalFormatting sqref="S15">
     <cfRule type="cellIs" priority="69" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>I17</formula>
+      <formula>I15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S22">
@@ -4309,14 +4297,14 @@
       <formula>I22</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S26">
+  <conditionalFormatting sqref="S27">
     <cfRule type="cellIs" priority="71" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>I26</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S30">
+      <formula>I27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S31">
     <cfRule type="cellIs" priority="72" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>I30</formula>
+      <formula>I31</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S33">
@@ -4324,63 +4312,62 @@
       <formula>I33</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="S34">
+    <cfRule type="cellIs" priority="74" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>I34</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="S35">
-    <cfRule type="cellIs" priority="74" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="75" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>I35</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S9">
-    <cfRule type="cellIs" priority="75" operator="lessThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>I9</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="O7" r:id="rId2" display="Link"/>
     <hyperlink ref="AA7" r:id="rId3" display="Link"/>
     <hyperlink ref="O9" r:id="rId4" display="Link"/>
-    <hyperlink ref="U9" r:id="rId5" display="Link"/>
-    <hyperlink ref="AA9" r:id="rId6" display="Link"/>
-    <hyperlink ref="O10" r:id="rId7" display="Link"/>
-    <hyperlink ref="O11" r:id="rId8" display="Link"/>
-    <hyperlink ref="U11" r:id="rId9" display="Link"/>
-    <hyperlink ref="O12" r:id="rId10" display="Link"/>
-    <hyperlink ref="U12" r:id="rId11" display="Link"/>
-    <hyperlink ref="O13" r:id="rId12" display="Link"/>
-    <hyperlink ref="O14" r:id="rId13" display="Link"/>
-    <hyperlink ref="U14" r:id="rId14" display="Link"/>
-    <hyperlink ref="O15" r:id="rId15" display="Link"/>
+    <hyperlink ref="AA9" r:id="rId5" display="Link"/>
+    <hyperlink ref="O10" r:id="rId6" display="Link"/>
+    <hyperlink ref="O11" r:id="rId7" display="Link"/>
+    <hyperlink ref="U11" r:id="rId8" display="Link"/>
+    <hyperlink ref="O12" r:id="rId9" display="Link"/>
+    <hyperlink ref="U12" r:id="rId10" display="Link"/>
+    <hyperlink ref="O13" r:id="rId11" display="Link"/>
+    <hyperlink ref="O14" r:id="rId12" display="Link"/>
+    <hyperlink ref="U14" r:id="rId13" display="Link"/>
+    <hyperlink ref="O15" r:id="rId14" display="Link"/>
+    <hyperlink ref="U15" r:id="rId15" display="Link"/>
     <hyperlink ref="O16" r:id="rId16" display="Link"/>
     <hyperlink ref="O17" r:id="rId17" display="Link"/>
-    <hyperlink ref="U17" r:id="rId18" display="Link"/>
-    <hyperlink ref="AA17" r:id="rId19" display="Link"/>
-    <hyperlink ref="O18" r:id="rId20" display="Link"/>
-    <hyperlink ref="AA18" r:id="rId21" display="Link"/>
-    <hyperlink ref="O19" r:id="rId22" display="Link"/>
-    <hyperlink ref="O20" r:id="rId23" display="Link"/>
-    <hyperlink ref="O21" r:id="rId24" display="Link"/>
-    <hyperlink ref="O22" r:id="rId25" display="Link"/>
-    <hyperlink ref="U22" r:id="rId26" display="Link"/>
-    <hyperlink ref="AA22" r:id="rId27" display="Link"/>
-    <hyperlink ref="O23" r:id="rId28" display="Link"/>
-    <hyperlink ref="O24" r:id="rId29" display="Link"/>
-    <hyperlink ref="O25" r:id="rId30" display="Link"/>
-    <hyperlink ref="O26" r:id="rId31" display="Link"/>
-    <hyperlink ref="U26" r:id="rId32" display="Link"/>
-    <hyperlink ref="AA26" r:id="rId33" display="Link"/>
-    <hyperlink ref="O27" r:id="rId34" display="Link"/>
-    <hyperlink ref="O28" r:id="rId35" display="Link"/>
-    <hyperlink ref="O29" r:id="rId36" display="Link"/>
-    <hyperlink ref="O30" r:id="rId37" display="Link"/>
-    <hyperlink ref="U30" r:id="rId38" display="Link"/>
-    <hyperlink ref="O31" r:id="rId39" display="Link"/>
-    <hyperlink ref="O32" r:id="rId40" display="Link"/>
-    <hyperlink ref="AA32" r:id="rId41" display="Link"/>
-    <hyperlink ref="O33" r:id="rId42" display="Link"/>
-    <hyperlink ref="U33" r:id="rId43" display="Link"/>
-    <hyperlink ref="AA33" r:id="rId44" display="Link"/>
-    <hyperlink ref="O34" r:id="rId45" display="Link"/>
-    <hyperlink ref="AA34" r:id="rId46" display="Link"/>
-    <hyperlink ref="U35" r:id="rId47" display="Link"/>
+    <hyperlink ref="AA17" r:id="rId18" display="Link"/>
+    <hyperlink ref="O18" r:id="rId19" display="Link"/>
+    <hyperlink ref="AA18" r:id="rId20" display="Link"/>
+    <hyperlink ref="O19" r:id="rId21" display="Link"/>
+    <hyperlink ref="O20" r:id="rId22" display="Link"/>
+    <hyperlink ref="O21" r:id="rId23" display="Link"/>
+    <hyperlink ref="O22" r:id="rId24" display="Link"/>
+    <hyperlink ref="U22" r:id="rId25" display="Link"/>
+    <hyperlink ref="AA22" r:id="rId26" display="Link"/>
+    <hyperlink ref="O23" r:id="rId27" display="Link"/>
+    <hyperlink ref="O24" r:id="rId28" display="Link"/>
+    <hyperlink ref="O25" r:id="rId29" display="Link"/>
+    <hyperlink ref="O26" r:id="rId30" display="Link"/>
+    <hyperlink ref="AA26" r:id="rId31" display="Link"/>
+    <hyperlink ref="O27" r:id="rId32" display="Link"/>
+    <hyperlink ref="U27" r:id="rId33" display="Link"/>
+    <hyperlink ref="O28" r:id="rId34" display="Link"/>
+    <hyperlink ref="O29" r:id="rId35" display="Link"/>
+    <hyperlink ref="O30" r:id="rId36" display="Link"/>
+    <hyperlink ref="O31" r:id="rId37" display="Link"/>
+    <hyperlink ref="U31" r:id="rId38" display="Link"/>
+    <hyperlink ref="O32" r:id="rId39" display="Link"/>
+    <hyperlink ref="O33" r:id="rId40" display="Link"/>
+    <hyperlink ref="U33" r:id="rId41" display="Link"/>
+    <hyperlink ref="AA33" r:id="rId42" display="Link"/>
+    <hyperlink ref="O34" r:id="rId43" display="Link"/>
+    <hyperlink ref="U34" r:id="rId44" display="Link"/>
+    <hyperlink ref="AA34" r:id="rId45" display="Link"/>
+    <hyperlink ref="U35" r:id="rId46" display="Link"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4389,6 +4376,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <legacyDrawing r:id="rId48"/>
+  <legacyDrawing r:id="rId47"/>
 </worksheet>
 </file>
</xml_diff>